<commit_message>
Started normalization_rna module. Added rasterisation.
</commit_message>
<xml_diff>
--- a/datasets/10x_pbmc_datasets.xlsx
+++ b/datasets/10x_pbmc_datasets.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t xml:space="preserve">sample</t>
   </si>
@@ -92,6 +92,15 @@
   </si>
   <si>
     <t xml:space="preserve">ENSEMBL,NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pbmc_3k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">smartseq2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">datasets/10x_SmartSeq2_pbmc_GSE132044/counts/smartseq2/counts_table.tsv.gz</t>
   </si>
 </sst>
 </file>
@@ -188,13 +197,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.56"/>
   </cols>
@@ -281,6 +290,26 @@
       </c>
       <c r="I3" s="0" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>